<commit_message>
Wrote up README and other annotations.
</commit_message>
<xml_diff>
--- a/processed data/PPHS Summary.xlsx
+++ b/processed data/PPHS Summary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yeelongsiah/Desktop/Personal/PythonLearning/PPHS/processed data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4F4CFED-F648-F946-8ADB-373C1CD41EA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F99DCBB-39C4-F341-9711-27FD01686992}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -635,8 +635,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J42"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="180" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>